<commit_message>
added more enemies and their values
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Excel/Value/EnemyValue.xlsx
+++ b/Assets/StreamingAssets/Excel/Value/EnemyValue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNR Classes and Files\CS 425 - Software Engineering\Senior Projects - Game\CS425-426\Assets\StreamingAssets\Excel\Value\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7159E0E-5DD7-4CFE-B006-C8C036219826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C429DBD-4A5B-4DF8-B339-345A15E7116D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -69,6 +69,24 @@
   </si>
   <si>
     <t xml:space="preserve">Bite = 9, Claw = 7, Pounce = 12 </t>
+  </si>
+  <si>
+    <t>Swoop Bite = 8, Wing Slash = 6, Blood Drain = 6 (for 2 turns)</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>Bat</t>
+  </si>
+  <si>
+    <t>Gnaw = 7, Bite = 5</t>
+  </si>
+  <si>
+    <t>Four-Legged Zombie</t>
+  </si>
+  <si>
+    <t>Sweeping Claw = 16, Leech Bite = 12</t>
   </si>
 </sst>
 </file>
@@ -386,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +457,7 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>13</v>
@@ -472,6 +490,78 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>ROW()-2</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>ROW()-2</f>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>ROW()-2</f>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>